<commit_message>
Término da apresentação dos requisitos no wireframe e término da planilha de requisitos
</commit_message>
<xml_diff>
--- a/wireframe/requsitos-funcionais.xlsx
+++ b/wireframe/requsitos-funcionais.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Documents/Desenvolvimento/repositorios/fai.etanois.docs/wireframe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AE001E-A32A-1F44-BE84-F30FF5738FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF647F8-6EBF-F74D-821C-7332911E64EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{71CBD75D-2557-E541-AF42-3850A17A2D20}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="80">
   <si>
     <t>Requisitos funcionais - Etanóis</t>
   </si>
@@ -117,12 +117,6 @@
   </si>
   <si>
     <t>Inativar combutível preferido pelo usuário</t>
-  </si>
-  <si>
-    <t>Cadastrar distância máxima de busca por postos</t>
-  </si>
-  <si>
-    <t>Editar distância máxima de busca por postos</t>
   </si>
   <si>
     <t>Cadastrar CEP do usuário</t>
@@ -271,6 +265,27 @@
   </si>
   <si>
     <t>Realizar pagamento através de QR Code</t>
+  </si>
+  <si>
+    <t>Depositar Etacoins via transferência</t>
+  </si>
+  <si>
+    <t>Status (wireframe)</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Cadastrar distância máxima de busca por postos sem rotas</t>
+  </si>
+  <si>
+    <t>Editar distância máxima de busca por postos sem rotas</t>
+  </si>
+  <si>
+    <t>Cadastrar distância máxima de busca por postos com rotas</t>
+  </si>
+  <si>
+    <t>Editar distância máxima de busca por postos com rotas</t>
   </si>
 </sst>
 </file>
@@ -323,7 +338,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -694,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492400C7-F164-8F4F-9D0E-0974B6B73B6D}">
-  <dimension ref="B2:F58"/>
+  <dimension ref="B2:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,9 +751,10 @@
     <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +762,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -730,10 +776,13 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -747,10 +796,13 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -764,10 +816,13 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -781,10 +836,13 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -798,10 +856,13 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
@@ -815,10 +876,13 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>6</v>
       </c>
@@ -832,10 +896,10 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
@@ -849,10 +913,10 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>8</v>
       </c>
@@ -866,10 +930,10 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>9</v>
       </c>
@@ -883,10 +947,10 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>10</v>
       </c>
@@ -900,10 +964,10 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>11</v>
       </c>
@@ -917,10 +981,10 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>12</v>
       </c>
@@ -934,10 +998,10 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>13</v>
       </c>
@@ -951,10 +1015,10 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>14</v>
       </c>
@@ -968,10 +1032,13 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>15</v>
       </c>
@@ -985,10 +1052,13 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1002,15 +1072,18 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1019,15 +1092,18 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -1036,15 +1112,18 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1053,15 +1132,18 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
@@ -1070,15 +1152,18 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1087,32 +1172,38 @@
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -1121,197 +1212,233 @@
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="G29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>35</v>
       </c>
@@ -1319,353 +1446,467 @@
         <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E49" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E52" t="s">
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="G52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="G53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="G54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="G55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="G58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>60</v>
+      </c>
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="C60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>60</v>
+      </c>
+      <c r="G60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1675,16 +1916,16 @@
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:E1 B2 B59:E1048576 B3:F58">
-    <cfRule type="expression" dxfId="2" priority="6">
+  <conditionalFormatting sqref="B1:E1 B2 G3:G8 B3:F21 G17:G21 B62:E1048576 C24:F61 G24:G55 G58:G60 C22:G23 B22:B61">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$E1="Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1 B2 B59:E1048576 B3:F58">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B1:E1 B2 G3:G8 B3:F21 G17:G21 B62:E1048576 C24:F61 G24:G55 G58:G60 C22:G23 B22:B61">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E1="Desejável"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$E1="Importante"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>